<commit_message>
changes to switch pd.read_excel to openpyxl engine
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/distributions/design.xlsx
+++ b/tests/data/sensitivities/distributions/design.xlsx
@@ -5,14 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DesignSheet01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="DefaultValues" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>0 for base case velocity model, 1: alternative velocity model</t>
+          <t xml:space="preserve">0 for base case velocity model, 1: alternative velocity model</t>
         </r>
       </text>
     </comment>
@@ -44,7 +48,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Oil water contact in Aare, eastern part of field</t>
+          <t xml:space="preserve">Oil water contact in Aare, eastern part of field</t>
         </r>
       </text>
     </comment>
@@ -57,7 +61,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Gas fill degree in P2 structural high. 
+          <t xml:space="preserve">Gas fill degree in P2 structural high. 
 0: no gas in P2 area, 1: filled to spill between P2 and P1 area</t>
         </r>
       </text>
@@ -71,7 +75,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Choosing between 0: tight case, 0.5: base case, 1: open case for fault seal</t>
+          <t xml:space="preserve">Choosing between 0: tight case, 0.5: base case, 1: open case for fault seal</t>
         </r>
       </text>
     </comment>
@@ -84,7 +88,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Gas oil relative permeabilityIleTofte</t>
+          <t xml:space="preserve">Gas oil relative permeabilityIleTofte</t>
         </r>
       </text>
     </comment>
@@ -93,189 +97,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="47">
   <si>
-    <t>REAL</t>
+    <t xml:space="preserve">REAL</t>
   </si>
   <si>
-    <t>SENSNAME</t>
+    <t xml:space="preserve">SENSNAME</t>
   </si>
   <si>
-    <t>SENSCASE</t>
+    <t xml:space="preserve">SENSCASE</t>
   </si>
   <si>
-    <t>RMS_SEED</t>
+    <t xml:space="preserve">RMS_SEED</t>
   </si>
   <si>
-    <t>COHIBA_MODE</t>
+    <t xml:space="preserve">COHIBA_MODE</t>
   </si>
   <si>
-    <t>RAND_VEL_MODEL</t>
+    <t xml:space="preserve">RAND_VEL_MODEL</t>
   </si>
   <si>
-    <t>OWCAEAST</t>
+    <t xml:space="preserve">OWCAEAST</t>
   </si>
   <si>
-    <t>GP2FILL</t>
+    <t xml:space="preserve">GP2FILL</t>
   </si>
   <si>
-    <t>FAULTSEAL</t>
+    <t xml:space="preserve">FAULTSEAL</t>
   </si>
   <si>
-    <t>RELP_GO_ILETOFTE</t>
+    <t xml:space="preserve">RELP_GO_ILETOFTE</t>
   </si>
   <si>
-    <t>rms_seed</t>
+    <t xml:space="preserve">rms_seed</t>
   </si>
   <si>
-    <t>P10_P90</t>
+    <t xml:space="preserve">P10_P90</t>
   </si>
   <si>
-    <t>PREDICTION</t>
+    <t xml:space="preserve">PREDICTION</t>
   </si>
   <si>
-    <t>hum_seed</t>
+    <t xml:space="preserve">hum_seed</t>
   </si>
   <si>
-    <t>SIMULATION</t>
+    <t xml:space="preserve">SIMULATION</t>
   </si>
   <si>
-    <t>velmodel</t>
+    <t xml:space="preserve">velmodel</t>
   </si>
   <si>
-    <t>alternative</t>
+    <t xml:space="preserve">alternative</t>
   </si>
   <si>
-    <t>owc_aeast</t>
+    <t xml:space="preserve">owc_aeast</t>
   </si>
   <si>
-    <t>shallow</t>
+    <t xml:space="preserve">shallow</t>
   </si>
   <si>
-    <t>deep</t>
+    <t xml:space="preserve">deep</t>
   </si>
   <si>
-    <t>gas_fraction</t>
+    <t xml:space="preserve">gas_fraction</t>
   </si>
   <si>
-    <t>no_fill</t>
+    <t xml:space="preserve">no_fill</t>
   </si>
   <si>
-    <t>filled</t>
+    <t xml:space="preserve">filled</t>
   </si>
   <si>
-    <t>fault_seal</t>
+    <t xml:space="preserve">fault_seal</t>
   </si>
   <si>
-    <t>open</t>
+    <t xml:space="preserve">open</t>
   </si>
   <si>
-    <t>tight</t>
+    <t xml:space="preserve">tight</t>
   </si>
   <si>
-    <t>relp_go</t>
+    <t xml:space="preserve">relp_go</t>
   </si>
   <si>
-    <t>lc</t>
+    <t xml:space="preserve">lc</t>
   </si>
   <si>
-    <t>hc</t>
+    <t xml:space="preserve">hc</t>
   </si>
   <si>
-    <t>WPIMULT_P_4S</t>
+    <t xml:space="preserve">WPIMULT_P_4S</t>
   </si>
   <si>
-    <t>WPIMULT_P_4M</t>
+    <t xml:space="preserve">WPIMULT_P_4M</t>
   </si>
   <si>
-    <t>MULTFLT_7</t>
+    <t xml:space="preserve">MULTFLT_7</t>
   </si>
   <si>
-    <t>MULTFLT_8N</t>
+    <t xml:space="preserve">MULTFLT_8N</t>
   </si>
   <si>
-    <t>MULTFLT_18</t>
+    <t xml:space="preserve">MULTFLT_18</t>
   </si>
   <si>
-    <t>MULTFLT_15</t>
+    <t xml:space="preserve">MULTFLT_15</t>
   </si>
   <si>
-    <t>MULTFLT_17</t>
+    <t xml:space="preserve">MULTFLT_17</t>
   </si>
   <si>
-    <t>FAULT_MIG_UNC</t>
+    <t xml:space="preserve">FAULT_MIG_UNC</t>
   </si>
   <si>
-    <t>MF001_SHIFT</t>
+    <t xml:space="preserve">MF001_SHIFT</t>
   </si>
   <si>
-    <t>MF002_SHIFT</t>
+    <t xml:space="preserve">MF002_SHIFT</t>
   </si>
   <si>
-    <t>OWCITTAW</t>
+    <t xml:space="preserve">OWCITTAW</t>
   </si>
   <si>
-    <t>GOCP1</t>
+    <t xml:space="preserve">GOCP1</t>
   </si>
   <si>
-    <t>MINK_AA_TZ</t>
+    <t xml:space="preserve">MINK_AA_TZ</t>
   </si>
   <si>
-    <t>PERM_P1R4</t>
+    <t xml:space="preserve">PERM_P1R4</t>
   </si>
   <si>
-    <t>PERM_5679</t>
+    <t xml:space="preserve">PERM_5679</t>
   </si>
   <si>
-    <t>RELP_GO_AARE</t>
+    <t xml:space="preserve">RELP_GO_AARE</t>
   </si>
   <si>
-    <t>RELP_OW_ILETOFTE</t>
+    <t xml:space="preserve">RELP_OW_ILETOFTE</t>
   </si>
   <si>
-    <t>RELP_OW_AARE</t>
-  </si>
-  <si>
-    <t>Required columns in DesignSheet01 are:</t>
-  </si>
-  <si>
-    <t>Realisation number: Integers 0,1,2,3,4.....</t>
-  </si>
-  <si>
-    <t>Name of sensitivity. 'Seed' spcifies that only RMS seed is varying, and this is the reference ensemble used in the Tornado Plot.</t>
-  </si>
-  <si>
-    <t>Any string can be given as name for other sensitivities</t>
-  </si>
-  <si>
-    <t>Specifying monte carlo sensitivities or low case/high case for each SENSNAME</t>
-  </si>
-  <si>
-    <t>'P10_P90'</t>
-  </si>
-  <si>
-    <t>is a predefined code to tell that this is a montecarlo sensitivity where P10 and P90 should be calculated and plotted in the Tornado</t>
-  </si>
-  <si>
-    <t>Any other string is valid as SENSCASE for scalar sensitivities: 'low_case', 'high_case', 'deep_contacts' , 'shallow_contacts' etc</t>
-  </si>
-  <si>
-    <t>Only one senscase for monte carlo sensitivities</t>
-  </si>
-  <si>
-    <t>One or two senscases for scalar sensitivities</t>
-  </si>
-  <si>
-    <t>Optional columns:</t>
-  </si>
-  <si>
-    <t>Optional parameter. RMS_SEED can also be given as separate file</t>
-  </si>
-  <si>
-    <t>For better readability recommending to use 1000, 1001, 1002,...</t>
-  </si>
-  <si>
-    <t>Repeat the seeds for each SENSCASE</t>
+    <t xml:space="preserve">RELP_OW_AARE</t>
   </si>
 </sst>
 </file>
@@ -283,7 +245,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -464,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,10 +793,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -914,27 +872,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:111"/>
+  <dimension ref="A1:AMJ111"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="19.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="9.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="12.4642857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,7 +4459,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4518,14 +4475,13 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4731,118 +4687,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="92" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="92" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="92" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Compatibility with xlrd 1.2 and 2.0, and pandas 1.x  (#94)
* changes to switch pd.read_excel to openpyxl engine

Co-authored-by: Trine Alsos <tral@statoil.com>
</commit_message>
<xml_diff>
--- a/tests/data/sensitivities/distributions/design.xlsx
+++ b/tests/data/sensitivities/distributions/design.xlsx
@@ -5,14 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DesignSheet01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="DefaultValues" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>0 for base case velocity model, 1: alternative velocity model</t>
+          <t xml:space="preserve">0 for base case velocity model, 1: alternative velocity model</t>
         </r>
       </text>
     </comment>
@@ -44,7 +48,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Oil water contact in Aare, eastern part of field</t>
+          <t xml:space="preserve">Oil water contact in Aare, eastern part of field</t>
         </r>
       </text>
     </comment>
@@ -57,7 +61,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Gas fill degree in P2 structural high. 
+          <t xml:space="preserve">Gas fill degree in P2 structural high. 
 0: no gas in P2 area, 1: filled to spill between P2 and P1 area</t>
         </r>
       </text>
@@ -71,7 +75,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Choosing between 0: tight case, 0.5: base case, 1: open case for fault seal</t>
+          <t xml:space="preserve">Choosing between 0: tight case, 0.5: base case, 1: open case for fault seal</t>
         </r>
       </text>
     </comment>
@@ -84,7 +88,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Gas oil relative permeabilityIleTofte</t>
+          <t xml:space="preserve">Gas oil relative permeabilityIleTofte</t>
         </r>
       </text>
     </comment>
@@ -93,189 +97,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="47">
   <si>
-    <t>REAL</t>
+    <t xml:space="preserve">REAL</t>
   </si>
   <si>
-    <t>SENSNAME</t>
+    <t xml:space="preserve">SENSNAME</t>
   </si>
   <si>
-    <t>SENSCASE</t>
+    <t xml:space="preserve">SENSCASE</t>
   </si>
   <si>
-    <t>RMS_SEED</t>
+    <t xml:space="preserve">RMS_SEED</t>
   </si>
   <si>
-    <t>COHIBA_MODE</t>
+    <t xml:space="preserve">COHIBA_MODE</t>
   </si>
   <si>
-    <t>RAND_VEL_MODEL</t>
+    <t xml:space="preserve">RAND_VEL_MODEL</t>
   </si>
   <si>
-    <t>OWCAEAST</t>
+    <t xml:space="preserve">OWCAEAST</t>
   </si>
   <si>
-    <t>GP2FILL</t>
+    <t xml:space="preserve">GP2FILL</t>
   </si>
   <si>
-    <t>FAULTSEAL</t>
+    <t xml:space="preserve">FAULTSEAL</t>
   </si>
   <si>
-    <t>RELP_GO_ILETOFTE</t>
+    <t xml:space="preserve">RELP_GO_ILETOFTE</t>
   </si>
   <si>
-    <t>rms_seed</t>
+    <t xml:space="preserve">rms_seed</t>
   </si>
   <si>
-    <t>P10_P90</t>
+    <t xml:space="preserve">P10_P90</t>
   </si>
   <si>
-    <t>PREDICTION</t>
+    <t xml:space="preserve">PREDICTION</t>
   </si>
   <si>
-    <t>hum_seed</t>
+    <t xml:space="preserve">hum_seed</t>
   </si>
   <si>
-    <t>SIMULATION</t>
+    <t xml:space="preserve">SIMULATION</t>
   </si>
   <si>
-    <t>velmodel</t>
+    <t xml:space="preserve">velmodel</t>
   </si>
   <si>
-    <t>alternative</t>
+    <t xml:space="preserve">alternative</t>
   </si>
   <si>
-    <t>owc_aeast</t>
+    <t xml:space="preserve">owc_aeast</t>
   </si>
   <si>
-    <t>shallow</t>
+    <t xml:space="preserve">shallow</t>
   </si>
   <si>
-    <t>deep</t>
+    <t xml:space="preserve">deep</t>
   </si>
   <si>
-    <t>gas_fraction</t>
+    <t xml:space="preserve">gas_fraction</t>
   </si>
   <si>
-    <t>no_fill</t>
+    <t xml:space="preserve">no_fill</t>
   </si>
   <si>
-    <t>filled</t>
+    <t xml:space="preserve">filled</t>
   </si>
   <si>
-    <t>fault_seal</t>
+    <t xml:space="preserve">fault_seal</t>
   </si>
   <si>
-    <t>open</t>
+    <t xml:space="preserve">open</t>
   </si>
   <si>
-    <t>tight</t>
+    <t xml:space="preserve">tight</t>
   </si>
   <si>
-    <t>relp_go</t>
+    <t xml:space="preserve">relp_go</t>
   </si>
   <si>
-    <t>lc</t>
+    <t xml:space="preserve">lc</t>
   </si>
   <si>
-    <t>hc</t>
+    <t xml:space="preserve">hc</t>
   </si>
   <si>
-    <t>WPIMULT_P_4S</t>
+    <t xml:space="preserve">WPIMULT_P_4S</t>
   </si>
   <si>
-    <t>WPIMULT_P_4M</t>
+    <t xml:space="preserve">WPIMULT_P_4M</t>
   </si>
   <si>
-    <t>MULTFLT_7</t>
+    <t xml:space="preserve">MULTFLT_7</t>
   </si>
   <si>
-    <t>MULTFLT_8N</t>
+    <t xml:space="preserve">MULTFLT_8N</t>
   </si>
   <si>
-    <t>MULTFLT_18</t>
+    <t xml:space="preserve">MULTFLT_18</t>
   </si>
   <si>
-    <t>MULTFLT_15</t>
+    <t xml:space="preserve">MULTFLT_15</t>
   </si>
   <si>
-    <t>MULTFLT_17</t>
+    <t xml:space="preserve">MULTFLT_17</t>
   </si>
   <si>
-    <t>FAULT_MIG_UNC</t>
+    <t xml:space="preserve">FAULT_MIG_UNC</t>
   </si>
   <si>
-    <t>MF001_SHIFT</t>
+    <t xml:space="preserve">MF001_SHIFT</t>
   </si>
   <si>
-    <t>MF002_SHIFT</t>
+    <t xml:space="preserve">MF002_SHIFT</t>
   </si>
   <si>
-    <t>OWCITTAW</t>
+    <t xml:space="preserve">OWCITTAW</t>
   </si>
   <si>
-    <t>GOCP1</t>
+    <t xml:space="preserve">GOCP1</t>
   </si>
   <si>
-    <t>MINK_AA_TZ</t>
+    <t xml:space="preserve">MINK_AA_TZ</t>
   </si>
   <si>
-    <t>PERM_P1R4</t>
+    <t xml:space="preserve">PERM_P1R4</t>
   </si>
   <si>
-    <t>PERM_5679</t>
+    <t xml:space="preserve">PERM_5679</t>
   </si>
   <si>
-    <t>RELP_GO_AARE</t>
+    <t xml:space="preserve">RELP_GO_AARE</t>
   </si>
   <si>
-    <t>RELP_OW_ILETOFTE</t>
+    <t xml:space="preserve">RELP_OW_ILETOFTE</t>
   </si>
   <si>
-    <t>RELP_OW_AARE</t>
-  </si>
-  <si>
-    <t>Required columns in DesignSheet01 are:</t>
-  </si>
-  <si>
-    <t>Realisation number: Integers 0,1,2,3,4.....</t>
-  </si>
-  <si>
-    <t>Name of sensitivity. 'Seed' spcifies that only RMS seed is varying, and this is the reference ensemble used in the Tornado Plot.</t>
-  </si>
-  <si>
-    <t>Any string can be given as name for other sensitivities</t>
-  </si>
-  <si>
-    <t>Specifying monte carlo sensitivities or low case/high case for each SENSNAME</t>
-  </si>
-  <si>
-    <t>'P10_P90'</t>
-  </si>
-  <si>
-    <t>is a predefined code to tell that this is a montecarlo sensitivity where P10 and P90 should be calculated and plotted in the Tornado</t>
-  </si>
-  <si>
-    <t>Any other string is valid as SENSCASE for scalar sensitivities: 'low_case', 'high_case', 'deep_contacts' , 'shallow_contacts' etc</t>
-  </si>
-  <si>
-    <t>Only one senscase for monte carlo sensitivities</t>
-  </si>
-  <si>
-    <t>One or two senscases for scalar sensitivities</t>
-  </si>
-  <si>
-    <t>Optional columns:</t>
-  </si>
-  <si>
-    <t>Optional parameter. RMS_SEED can also be given as separate file</t>
-  </si>
-  <si>
-    <t>For better readability recommending to use 1000, 1001, 1002,...</t>
-  </si>
-  <si>
-    <t>Repeat the seeds for each SENSCASE</t>
+    <t xml:space="preserve">RELP_OW_AARE</t>
   </si>
 </sst>
 </file>
@@ -283,7 +245,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -464,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,10 +793,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -914,27 +872,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:111"/>
+  <dimension ref="A1:AMJ111"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="19.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="9.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="12.4642857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="12.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,7 +4459,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4518,14 +4475,13 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4731,118 +4687,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="92" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="92" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="92" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>